<commit_message>
100 Test Cases Implemented
</commit_message>
<xml_diff>
--- a/Amazon/DataTest/AmazonData.xlsx
+++ b/Amazon/DataTest/AmazonData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706D4085-3512-F949-9AF1-719AD71EF5FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>ProductName</t>
-  </si>
-  <si>
-    <t>Hand sanitizer</t>
   </si>
   <si>
     <t>T-shirt</t>
@@ -278,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -608,66 +606,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -676,73 +674,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -751,358 +749,358 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
       </c>
       <c r="C2">
         <v>45345345</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3">
         <v>25810</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
       </c>
       <c r="C3">
         <v>45345346</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
         <v>25811</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
       </c>
       <c r="C4">
         <v>45345347</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3">
         <v>25812</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
       </c>
       <c r="C5">
         <v>45345348</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3">
         <v>25813</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
       </c>
       <c r="C6">
         <v>45345349</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3">
         <v>25814</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
       </c>
       <c r="C7">
         <v>45345350</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3">
         <v>25815</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
       </c>
       <c r="C8">
         <v>45345351</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3">
         <v>25816</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
       </c>
       <c r="C9">
         <v>45345352</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3">
         <v>25817</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
       </c>
       <c r="C10">
         <v>45345353</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3">
         <v>25818</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
         <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>67</v>
       </c>
       <c r="C11">
         <v>45345354</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3">
         <v>25819</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
       </c>
       <c r="C12">
         <v>45345355</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="3">
         <v>25820</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
       </c>
       <c r="C13">
         <v>45345356</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="3">
         <v>25821</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
       </c>
       <c r="C14">
         <v>45345357</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3">
         <v>25822</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
         <v>74</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
       </c>
       <c r="C15">
         <v>45345358</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="3">
         <v>25823</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
         <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>77</v>
       </c>
       <c r="C16">
         <v>45345359</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="3">
         <v>25824</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
         <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>80</v>
       </c>
       <c r="C17">
         <v>45345360</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" s="3">
         <v>25825</v>
@@ -1110,22 +1108,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D15" r:id="rId9"/>
-    <hyperlink ref="D10" r:id="rId10"/>
-    <hyperlink ref="D16" r:id="rId11"/>
-    <hyperlink ref="D11" r:id="rId12"/>
-    <hyperlink ref="D17" r:id="rId13" display="james7@gmail.com"/>
-    <hyperlink ref="D12" r:id="rId14"/>
-    <hyperlink ref="D13" r:id="rId15"/>
-    <hyperlink ref="D14" r:id="rId16"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="D11" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="D17" r:id="rId13" display="james7@gmail.com" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="D12" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="D13" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="D14" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>